<commit_message>
No hay productos reconocidos que tengan las dos palabras claves
</commit_message>
<xml_diff>
--- a/BDCartasControl.xlsx
+++ b/BDCartasControl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\Documents\LEONARDO\CAR\CODIGOS\WebScraping MinCiencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0894AA-E5CB-4E96-9C5E-5BEC18A0DD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C729F7-3EA6-4B64-B9D5-6E59C856AD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,16 +498,16 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.44140625" customWidth="1"/>
-    <col min="2" max="2" width="50.33203125" customWidth="1"/>
+    <col min="1" max="1" width="91.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -523,7 +523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -539,7 +539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -547,7 +547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -563,7 +563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -571,63 +571,63 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
     </row>

</xml_diff>